<commit_message>
Remove the manual addition of Eday mrros from the ignore list in order to allow the production of Eday mrros by IFS #708.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmip6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmip6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6438" uniqueCount="1873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6417" uniqueCount="1868">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -4597,18 +4597,6 @@
     <t xml:space="preserve">Fraction of soil moisture mass in the liquid phase in each user-defined soil layer (3D variable)</t>
   </si>
   <si>
-    <t xml:space="preserve">mrros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Runoff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lars, Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The total surface run off leaving the land portion of the grid cell (excluding drainage through the base of the soil model).</t>
-  </si>
-  <si>
     <t xml:space="preserve">nudgincsm</t>
   </si>
   <si>
@@ -5495,9 +5483,6 @@
   </si>
   <si>
     <t xml:space="preserve">CMIP,OMIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AerChemMIP,C4MIP,CDRMIP,CFMIP,CMIP,FAFMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,LUMIP,PMIP,RFMIP,VIACSAB,VolMIP</t>
   </si>
   <si>
     <t xml:space="preserve">o3</t>
@@ -5758,8 +5743,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A622" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H643" activeCellId="0" sqref="H643"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A548" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A568" activeCellId="0" sqref="A568"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5773,7 +5758,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -24344,7 +24329,7 @@
         <v>974</v>
       </c>
       <c r="B568" s="0" t="s">
-        <v>1525</v>
+        <v>1212</v>
       </c>
       <c r="C568" s="0" t="s">
         <v>13</v>
@@ -24353,22 +24338,22 @@
         <v>151</v>
       </c>
       <c r="E568" s="0" t="s">
-        <v>1526</v>
+        <v>1213</v>
       </c>
       <c r="F568" s="0" t="s">
-        <v>153</v>
+        <v>28</v>
       </c>
       <c r="G568" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H568" s="0" t="s">
-        <v>1141</v>
+        <v>1463</v>
       </c>
       <c r="I568" s="0" t="s">
-        <v>1527</v>
+        <v>1464</v>
       </c>
       <c r="J568" s="0" t="s">
-        <v>1528</v>
+        <v>1216</v>
       </c>
       <c r="K568" s="0" t="s">
         <v>20</v>
@@ -24379,7 +24364,7 @@
         <v>974</v>
       </c>
       <c r="B569" s="0" t="s">
-        <v>1212</v>
+        <v>1525</v>
       </c>
       <c r="C569" s="0" t="s">
         <v>13</v>
@@ -24388,7 +24373,7 @@
         <v>151</v>
       </c>
       <c r="E569" s="0" t="s">
-        <v>1213</v>
+        <v>1526</v>
       </c>
       <c r="F569" s="0" t="s">
         <v>28</v>
@@ -24403,7 +24388,7 @@
         <v>1464</v>
       </c>
       <c r="J569" s="0" t="s">
-        <v>1216</v>
+        <v>1527</v>
       </c>
       <c r="K569" s="0" t="s">
         <v>20</v>
@@ -24414,7 +24399,7 @@
         <v>974</v>
       </c>
       <c r="B570" s="0" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="C570" s="0" t="s">
         <v>13</v>
@@ -24423,7 +24408,7 @@
         <v>151</v>
       </c>
       <c r="E570" s="0" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="F570" s="0" t="s">
         <v>28</v>
@@ -24438,7 +24423,7 @@
         <v>1464</v>
       </c>
       <c r="J570" s="0" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="K570" s="0" t="s">
         <v>20</v>
@@ -24449,7 +24434,7 @@
         <v>974</v>
       </c>
       <c r="B571" s="0" t="s">
-        <v>1532</v>
+        <v>1049</v>
       </c>
       <c r="C571" s="0" t="s">
         <v>13</v>
@@ -24458,22 +24443,22 @@
         <v>151</v>
       </c>
       <c r="E571" s="0" t="s">
-        <v>1533</v>
+        <v>1050</v>
       </c>
       <c r="F571" s="0" t="s">
-        <v>28</v>
+        <v>153</v>
       </c>
       <c r="G571" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H571" s="0" t="s">
-        <v>1463</v>
+        <v>1051</v>
       </c>
       <c r="I571" s="0" t="s">
-        <v>1464</v>
+        <v>56</v>
       </c>
       <c r="J571" s="0" t="s">
-        <v>1534</v>
+        <v>775</v>
       </c>
       <c r="K571" s="0" t="s">
         <v>20</v>
@@ -24484,7 +24469,7 @@
         <v>974</v>
       </c>
       <c r="B572" s="0" t="s">
-        <v>1049</v>
+        <v>1531</v>
       </c>
       <c r="C572" s="0" t="s">
         <v>13</v>
@@ -24493,22 +24478,22 @@
         <v>151</v>
       </c>
       <c r="E572" s="0" t="s">
-        <v>1050</v>
+        <v>1532</v>
       </c>
       <c r="F572" s="0" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="G572" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H572" s="0" t="s">
-        <v>1051</v>
+        <v>1460</v>
       </c>
       <c r="I572" s="0" t="s">
-        <v>56</v>
+        <v>1215</v>
       </c>
       <c r="J572" s="0" t="s">
-        <v>775</v>
+        <v>1533</v>
       </c>
       <c r="K572" s="0" t="s">
         <v>20</v>
@@ -24519,7 +24504,7 @@
         <v>974</v>
       </c>
       <c r="B573" s="0" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="C573" s="0" t="s">
         <v>13</v>
@@ -24528,7 +24513,7 @@
         <v>151</v>
       </c>
       <c r="E573" s="0" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="F573" s="0" t="s">
         <v>13</v>
@@ -24543,7 +24528,7 @@
         <v>1215</v>
       </c>
       <c r="J573" s="0" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="K573" s="0" t="s">
         <v>20</v>
@@ -24554,7 +24539,7 @@
         <v>974</v>
       </c>
       <c r="B574" s="0" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="C574" s="0" t="s">
         <v>13</v>
@@ -24563,22 +24548,22 @@
         <v>151</v>
       </c>
       <c r="E574" s="0" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="F574" s="0" t="s">
-        <v>13</v>
+        <v>153</v>
       </c>
       <c r="G574" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H574" s="0" t="s">
-        <v>1460</v>
+        <v>1478</v>
       </c>
       <c r="I574" s="0" t="s">
         <v>1215</v>
       </c>
       <c r="J574" s="0" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="K574" s="0" t="s">
         <v>20</v>
@@ -24589,7 +24574,7 @@
         <v>974</v>
       </c>
       <c r="B575" s="0" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="C575" s="0" t="s">
         <v>13</v>
@@ -24598,10 +24583,10 @@
         <v>151</v>
       </c>
       <c r="E575" s="0" t="s">
+        <v>1541</v>
+      </c>
+      <c r="F575" s="0" t="s">
         <v>1542</v>
-      </c>
-      <c r="F575" s="0" t="s">
-        <v>153</v>
       </c>
       <c r="G575" s="0" t="n">
         <v>0</v>
@@ -24636,7 +24621,7 @@
         <v>1545</v>
       </c>
       <c r="F576" s="0" t="s">
-        <v>1546</v>
+        <v>1542</v>
       </c>
       <c r="G576" s="0" t="n">
         <v>0</v>
@@ -24648,7 +24633,7 @@
         <v>1215</v>
       </c>
       <c r="J576" s="0" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="K576" s="0" t="s">
         <v>20</v>
@@ -24659,7 +24644,7 @@
         <v>974</v>
       </c>
       <c r="B577" s="0" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C577" s="0" t="s">
         <v>13</v>
@@ -24668,22 +24653,22 @@
         <v>151</v>
       </c>
       <c r="E577" s="0" t="s">
+        <v>1548</v>
+      </c>
+      <c r="F577" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G577" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H577" s="0" t="s">
+        <v>1463</v>
+      </c>
+      <c r="I577" s="0" t="s">
+        <v>1464</v>
+      </c>
+      <c r="J577" s="0" t="s">
         <v>1549</v>
-      </c>
-      <c r="F577" s="0" t="s">
-        <v>1546</v>
-      </c>
-      <c r="G577" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H577" s="0" t="s">
-        <v>1478</v>
-      </c>
-      <c r="I577" s="0" t="s">
-        <v>1215</v>
-      </c>
-      <c r="J577" s="0" t="s">
-        <v>1550</v>
       </c>
       <c r="K577" s="0" t="s">
         <v>20</v>
@@ -24694,7 +24679,7 @@
         <v>974</v>
       </c>
       <c r="B578" s="0" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C578" s="0" t="s">
         <v>13</v>
@@ -24703,22 +24688,22 @@
         <v>151</v>
       </c>
       <c r="E578" s="0" t="s">
+        <v>1551</v>
+      </c>
+      <c r="F578" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="G578" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H578" s="0" t="s">
+        <v>1505</v>
+      </c>
+      <c r="I578" s="0" t="s">
+        <v>1215</v>
+      </c>
+      <c r="J578" s="0" t="s">
         <v>1552</v>
-      </c>
-      <c r="F578" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G578" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H578" s="0" t="s">
-        <v>1463</v>
-      </c>
-      <c r="I578" s="0" t="s">
-        <v>1464</v>
-      </c>
-      <c r="J578" s="0" t="s">
-        <v>1553</v>
       </c>
       <c r="K578" s="0" t="s">
         <v>20</v>
@@ -24729,7 +24714,7 @@
         <v>974</v>
       </c>
       <c r="B579" s="0" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="C579" s="0" t="s">
         <v>13</v>
@@ -24738,7 +24723,7 @@
         <v>151</v>
       </c>
       <c r="E579" s="0" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F579" s="0" t="s">
         <v>153</v>
@@ -24747,13 +24732,13 @@
         <v>0</v>
       </c>
       <c r="H579" s="0" t="s">
-        <v>1505</v>
+        <v>1463</v>
       </c>
       <c r="I579" s="0" t="s">
-        <v>1215</v>
+        <v>1464</v>
       </c>
       <c r="J579" s="0" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="K579" s="0" t="s">
         <v>20</v>
@@ -24764,7 +24749,7 @@
         <v>974</v>
       </c>
       <c r="B580" s="0" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="C580" s="0" t="s">
         <v>13</v>
@@ -24773,7 +24758,7 @@
         <v>151</v>
       </c>
       <c r="E580" s="0" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="F580" s="0" t="s">
         <v>153</v>
@@ -24782,13 +24767,13 @@
         <v>0</v>
       </c>
       <c r="H580" s="0" t="s">
-        <v>1463</v>
+        <v>1505</v>
       </c>
       <c r="I580" s="0" t="s">
-        <v>1464</v>
+        <v>1215</v>
       </c>
       <c r="J580" s="0" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="K580" s="0" t="s">
         <v>20</v>
@@ -24799,7 +24784,7 @@
         <v>974</v>
       </c>
       <c r="B581" s="0" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="C581" s="0" t="s">
         <v>13</v>
@@ -24808,16 +24793,16 @@
         <v>151</v>
       </c>
       <c r="E581" s="0" t="s">
+        <v>1560</v>
+      </c>
+      <c r="F581" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G581" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H581" s="0" t="s">
         <v>1561</v>
-      </c>
-      <c r="F581" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="G581" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H581" s="0" t="s">
-        <v>1505</v>
       </c>
       <c r="I581" s="0" t="s">
         <v>1215</v>
@@ -24881,19 +24866,19 @@
         <v>1568</v>
       </c>
       <c r="F583" s="0" t="s">
-        <v>28</v>
+        <v>852</v>
       </c>
       <c r="G583" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H583" s="0" t="s">
+        <v>1463</v>
+      </c>
+      <c r="I583" s="0" t="s">
+        <v>1464</v>
+      </c>
+      <c r="J583" s="0" t="s">
         <v>1569</v>
-      </c>
-      <c r="I583" s="0" t="s">
-        <v>1215</v>
-      </c>
-      <c r="J583" s="0" t="s">
-        <v>1570</v>
       </c>
       <c r="K583" s="0" t="s">
         <v>20</v>
@@ -24904,7 +24889,7 @@
         <v>974</v>
       </c>
       <c r="B584" s="0" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="C584" s="0" t="s">
         <v>13</v>
@@ -24913,7 +24898,7 @@
         <v>151</v>
       </c>
       <c r="E584" s="0" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="F584" s="0" t="s">
         <v>852</v>
@@ -24928,7 +24913,7 @@
         <v>1464</v>
       </c>
       <c r="J584" s="0" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="K584" s="0" t="s">
         <v>20</v>
@@ -24939,7 +24924,7 @@
         <v>974</v>
       </c>
       <c r="B585" s="0" t="s">
-        <v>1574</v>
+        <v>1364</v>
       </c>
       <c r="C585" s="0" t="s">
         <v>13</v>
@@ -24948,79 +24933,79 @@
         <v>151</v>
       </c>
       <c r="E585" s="0" t="s">
-        <v>1575</v>
+        <v>1365</v>
       </c>
       <c r="F585" s="0" t="s">
-        <v>852</v>
+        <v>41</v>
       </c>
       <c r="G585" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H585" s="0" t="s">
-        <v>1463</v>
+        <v>1478</v>
       </c>
       <c r="I585" s="0" t="s">
-        <v>1464</v>
+        <v>1215</v>
       </c>
       <c r="J585" s="0" t="s">
-        <v>1576</v>
+        <v>1367</v>
       </c>
       <c r="K585" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A586" s="0" t="s">
-        <v>974</v>
-      </c>
-      <c r="B586" s="0" t="s">
-        <v>1364</v>
-      </c>
-      <c r="C586" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D586" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="E586" s="0" t="s">
-        <v>1365</v>
-      </c>
-      <c r="F586" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G586" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H586" s="0" t="s">
-        <v>1478</v>
-      </c>
-      <c r="I586" s="0" t="s">
-        <v>1215</v>
-      </c>
-      <c r="J586" s="0" t="s">
-        <v>1367</v>
-      </c>
-      <c r="K586" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
+    <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A588" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="B588" s="0" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C588" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D588" s="0" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E588" s="0" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F588" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="G588" s="0" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H588" s="0" t="s">
+        <v>1576</v>
+      </c>
+      <c r="I588" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="J588" s="0" t="s">
+        <v>1578</v>
+      </c>
+      <c r="K588" s="0" t="s">
+        <v>755</v>
+      </c>
+    </row>
     <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="0" t="s">
-        <v>740</v>
+        <v>1043</v>
       </c>
       <c r="B589" s="0" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
       <c r="C589" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D589" s="0" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="E589" s="0" t="s">
-        <v>1579</v>
+        <v>1575</v>
       </c>
       <c r="F589" s="0" t="s">
         <v>232</v>
@@ -25029,55 +25014,55 @@
         <v>1423</v>
       </c>
       <c r="H589" s="0" t="s">
-        <v>1580</v>
+        <v>1576</v>
       </c>
       <c r="I589" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J589" s="0" t="s">
-        <v>1582</v>
+        <v>1578</v>
       </c>
       <c r="K589" s="0" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A590" s="0" t="s">
-        <v>1043</v>
-      </c>
-      <c r="B590" s="0" t="s">
+    <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A592" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B592" s="0" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C592" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D592" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E592" s="0" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F592" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G592" s="0" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H592" s="0" t="s">
+        <v>1581</v>
+      </c>
+      <c r="I592" s="0" t="s">
         <v>1577</v>
       </c>
-      <c r="C590" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D590" s="0" t="s">
-        <v>1578</v>
-      </c>
-      <c r="E590" s="0" t="s">
-        <v>1579</v>
-      </c>
-      <c r="F590" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="G590" s="0" t="s">
-        <v>1423</v>
-      </c>
-      <c r="H590" s="0" t="s">
-        <v>1580</v>
-      </c>
-      <c r="I590" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="J590" s="0" t="s">
+      <c r="J592" s="0" t="s">
         <v>1582</v>
       </c>
-      <c r="K590" s="0" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="K592" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
     <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="0" t="s">
         <v>324</v>
@@ -25095,7 +25080,7 @@
         <v>1584</v>
       </c>
       <c r="F593" s="0" t="s">
-        <v>16</v>
+        <v>1127</v>
       </c>
       <c r="G593" s="0" t="s">
         <v>1423</v>
@@ -25104,7 +25089,7 @@
         <v>1585</v>
       </c>
       <c r="I593" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J593" s="0" t="s">
         <v>1586</v>
@@ -25139,7 +25124,7 @@
         <v>1589</v>
       </c>
       <c r="I594" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J594" s="0" t="s">
         <v>1590</v>
@@ -25165,7 +25150,7 @@
         <v>1592</v>
       </c>
       <c r="F595" s="0" t="s">
-        <v>1127</v>
+        <v>852</v>
       </c>
       <c r="G595" s="0" t="s">
         <v>1423</v>
@@ -25174,10 +25159,10 @@
         <v>1593</v>
       </c>
       <c r="I595" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J595" s="0" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="K595" s="0" t="s">
         <v>326</v>
@@ -25188,7 +25173,7 @@
         <v>324</v>
       </c>
       <c r="B596" s="0" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="C596" s="0" t="s">
         <v>13</v>
@@ -25197,22 +25182,22 @@
         <v>333</v>
       </c>
       <c r="E596" s="0" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="F596" s="0" t="s">
-        <v>852</v>
+        <v>296</v>
       </c>
       <c r="G596" s="0" t="s">
         <v>1423</v>
       </c>
       <c r="H596" s="0" t="s">
+        <v>1596</v>
+      </c>
+      <c r="I596" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="J596" s="0" t="s">
         <v>1597</v>
-      </c>
-      <c r="I596" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="J596" s="0" t="s">
-        <v>1596</v>
       </c>
       <c r="K596" s="0" t="s">
         <v>326</v>
@@ -25244,7 +25229,7 @@
         <v>1600</v>
       </c>
       <c r="I597" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J597" s="0" t="s">
         <v>1601</v>
@@ -25270,7 +25255,7 @@
         <v>1603</v>
       </c>
       <c r="F598" s="0" t="s">
-        <v>296</v>
+        <v>13</v>
       </c>
       <c r="G598" s="0" t="s">
         <v>1423</v>
@@ -25279,7 +25264,7 @@
         <v>1604</v>
       </c>
       <c r="I598" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J598" s="0" t="s">
         <v>1605</v>
@@ -25305,7 +25290,7 @@
         <v>1607</v>
       </c>
       <c r="F599" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G599" s="0" t="s">
         <v>1423</v>
@@ -25314,10 +25299,10 @@
         <v>1608</v>
       </c>
       <c r="I599" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J599" s="0" t="s">
-        <v>1609</v>
+        <v>990</v>
       </c>
       <c r="K599" s="0" t="s">
         <v>326</v>
@@ -25328,7 +25313,7 @@
         <v>324</v>
       </c>
       <c r="B600" s="0" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C600" s="0" t="s">
         <v>13</v>
@@ -25337,10 +25322,10 @@
         <v>333</v>
       </c>
       <c r="E600" s="0" t="s">
+        <v>1610</v>
+      </c>
+      <c r="F600" s="0" t="s">
         <v>1611</v>
-      </c>
-      <c r="F600" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="G600" s="0" t="s">
         <v>1423</v>
@@ -25349,10 +25334,10 @@
         <v>1612</v>
       </c>
       <c r="I600" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J600" s="0" t="s">
-        <v>990</v>
+        <v>1613</v>
       </c>
       <c r="K600" s="0" t="s">
         <v>326</v>
@@ -25363,7 +25348,7 @@
         <v>324</v>
       </c>
       <c r="B601" s="0" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="C601" s="0" t="s">
         <v>13</v>
@@ -25372,10 +25357,10 @@
         <v>333</v>
       </c>
       <c r="E601" s="0" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="F601" s="0" t="s">
-        <v>1615</v>
+        <v>41</v>
       </c>
       <c r="G601" s="0" t="s">
         <v>1423</v>
@@ -25384,7 +25369,7 @@
         <v>1616</v>
       </c>
       <c r="I601" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J601" s="0" t="s">
         <v>1617</v>
@@ -25410,7 +25395,7 @@
         <v>1619</v>
       </c>
       <c r="F602" s="0" t="s">
-        <v>41</v>
+        <v>232</v>
       </c>
       <c r="G602" s="0" t="s">
         <v>1423</v>
@@ -25419,7 +25404,7 @@
         <v>1620</v>
       </c>
       <c r="I602" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J602" s="0" t="s">
         <v>1621</v>
@@ -25433,16 +25418,16 @@
         <v>324</v>
       </c>
       <c r="B603" s="0" t="s">
-        <v>1622</v>
+        <v>1573</v>
       </c>
       <c r="C603" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D603" s="0" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="E603" s="0" t="s">
-        <v>1623</v>
+        <v>1575</v>
       </c>
       <c r="F603" s="0" t="s">
         <v>232</v>
@@ -25451,13 +25436,13 @@
         <v>1423</v>
       </c>
       <c r="H603" s="0" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="I603" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J603" s="0" t="s">
-        <v>1625</v>
+        <v>1578</v>
       </c>
       <c r="K603" s="0" t="s">
         <v>326</v>
@@ -25468,19 +25453,19 @@
         <v>324</v>
       </c>
       <c r="B604" s="0" t="s">
-        <v>1577</v>
+        <v>1623</v>
       </c>
       <c r="C604" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D604" s="0" t="s">
-        <v>345</v>
+        <v>1624</v>
       </c>
       <c r="E604" s="0" t="s">
-        <v>1579</v>
+        <v>1625</v>
       </c>
       <c r="F604" s="0" t="s">
-        <v>232</v>
+        <v>852</v>
       </c>
       <c r="G604" s="0" t="s">
         <v>1423</v>
@@ -25489,10 +25474,10 @@
         <v>1626</v>
       </c>
       <c r="I604" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J604" s="0" t="s">
-        <v>1582</v>
+        <v>1627</v>
       </c>
       <c r="K604" s="0" t="s">
         <v>326</v>
@@ -25503,13 +25488,13 @@
         <v>324</v>
       </c>
       <c r="B605" s="0" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="C605" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D605" s="0" t="s">
-        <v>1628</v>
+        <v>325</v>
       </c>
       <c r="E605" s="0" t="s">
         <v>1629</v>
@@ -25524,7 +25509,7 @@
         <v>1630</v>
       </c>
       <c r="I605" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J605" s="0" t="s">
         <v>1631</v>
@@ -25550,7 +25535,7 @@
         <v>1633</v>
       </c>
       <c r="F606" s="0" t="s">
-        <v>852</v>
+        <v>232</v>
       </c>
       <c r="G606" s="0" t="s">
         <v>1423</v>
@@ -25559,10 +25544,10 @@
         <v>1634</v>
       </c>
       <c r="I606" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J606" s="0" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="K606" s="0" t="s">
         <v>326</v>
@@ -25573,7 +25558,7 @@
         <v>324</v>
       </c>
       <c r="B607" s="0" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="C607" s="0" t="s">
         <v>13</v>
@@ -25582,7 +25567,7 @@
         <v>325</v>
       </c>
       <c r="E607" s="0" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="F607" s="0" t="s">
         <v>232</v>
@@ -25591,13 +25576,13 @@
         <v>1423</v>
       </c>
       <c r="H607" s="0" t="s">
+        <v>1637</v>
+      </c>
+      <c r="I607" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="J607" s="0" t="s">
         <v>1638</v>
-      </c>
-      <c r="I607" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="J607" s="0" t="s">
-        <v>1637</v>
       </c>
       <c r="K607" s="0" t="s">
         <v>326</v>
@@ -25614,25 +25599,25 @@
         <v>13</v>
       </c>
       <c r="D608" s="0" t="s">
-        <v>325</v>
+        <v>1640</v>
       </c>
       <c r="E608" s="0" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="F608" s="0" t="s">
-        <v>232</v>
+        <v>296</v>
       </c>
       <c r="G608" s="0" t="s">
         <v>1423</v>
       </c>
       <c r="H608" s="0" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="I608" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J608" s="0" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="K608" s="0" t="s">
         <v>326</v>
@@ -25643,13 +25628,13 @@
         <v>324</v>
       </c>
       <c r="B609" s="0" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="C609" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D609" s="0" t="s">
-        <v>1644</v>
+        <v>1640</v>
       </c>
       <c r="E609" s="0" t="s">
         <v>1645</v>
@@ -25664,7 +25649,7 @@
         <v>1646</v>
       </c>
       <c r="I609" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J609" s="0" t="s">
         <v>1647</v>
@@ -25684,7 +25669,7 @@
         <v>13</v>
       </c>
       <c r="D610" s="0" t="s">
-        <v>1644</v>
+        <v>1640</v>
       </c>
       <c r="E610" s="0" t="s">
         <v>1649</v>
@@ -25699,7 +25684,7 @@
         <v>1650</v>
       </c>
       <c r="I610" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J610" s="0" t="s">
         <v>1651</v>
@@ -25719,13 +25704,13 @@
         <v>13</v>
       </c>
       <c r="D611" s="0" t="s">
-        <v>1644</v>
+        <v>1624</v>
       </c>
       <c r="E611" s="0" t="s">
         <v>1653</v>
       </c>
       <c r="F611" s="0" t="s">
-        <v>296</v>
+        <v>16</v>
       </c>
       <c r="G611" s="0" t="s">
         <v>1423</v>
@@ -25734,10 +25719,10 @@
         <v>1654</v>
       </c>
       <c r="I611" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J611" s="0" t="s">
-        <v>1655</v>
+        <v>990</v>
       </c>
       <c r="K611" s="0" t="s">
         <v>326</v>
@@ -25748,31 +25733,31 @@
         <v>324</v>
       </c>
       <c r="B612" s="0" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C612" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D612" s="0" t="s">
+        <v>1624</v>
+      </c>
+      <c r="E612" s="0" t="s">
         <v>1656</v>
       </c>
-      <c r="C612" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D612" s="0" t="s">
-        <v>1628</v>
-      </c>
-      <c r="E612" s="0" t="s">
-        <v>1657</v>
-      </c>
       <c r="F612" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G612" s="0" t="s">
         <v>1423</v>
       </c>
       <c r="H612" s="0" t="s">
+        <v>1657</v>
+      </c>
+      <c r="I612" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="J612" s="0" t="s">
         <v>1658</v>
-      </c>
-      <c r="I612" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="J612" s="0" t="s">
-        <v>990</v>
       </c>
       <c r="K612" s="0" t="s">
         <v>326</v>
@@ -25789,13 +25774,13 @@
         <v>13</v>
       </c>
       <c r="D613" s="0" t="s">
-        <v>1628</v>
+        <v>325</v>
       </c>
       <c r="E613" s="0" t="s">
         <v>1660</v>
       </c>
       <c r="F613" s="0" t="s">
-        <v>13</v>
+        <v>153</v>
       </c>
       <c r="G613" s="0" t="s">
         <v>1423</v>
@@ -25804,7 +25789,7 @@
         <v>1661</v>
       </c>
       <c r="I613" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J613" s="0" t="s">
         <v>1662</v>
@@ -25839,7 +25824,7 @@
         <v>1665</v>
       </c>
       <c r="I614" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J614" s="0" t="s">
         <v>1666</v>
@@ -25874,7 +25859,7 @@
         <v>1669</v>
       </c>
       <c r="I615" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J615" s="0" t="s">
         <v>1670</v>
@@ -25909,7 +25894,7 @@
         <v>1673</v>
       </c>
       <c r="I616" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J616" s="0" t="s">
         <v>1674</v>
@@ -25944,7 +25929,7 @@
         <v>1677</v>
       </c>
       <c r="I617" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J617" s="0" t="s">
         <v>1678</v>
@@ -25970,7 +25955,7 @@
         <v>1680</v>
       </c>
       <c r="F618" s="0" t="s">
-        <v>153</v>
+        <v>232</v>
       </c>
       <c r="G618" s="0" t="s">
         <v>1423</v>
@@ -25979,7 +25964,7 @@
         <v>1681</v>
       </c>
       <c r="I618" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J618" s="0" t="s">
         <v>1682</v>
@@ -26014,7 +25999,7 @@
         <v>1685</v>
       </c>
       <c r="I619" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J619" s="0" t="s">
         <v>1686</v>
@@ -26040,7 +26025,7 @@
         <v>1688</v>
       </c>
       <c r="F620" s="0" t="s">
-        <v>232</v>
+        <v>348</v>
       </c>
       <c r="G620" s="0" t="s">
         <v>1423</v>
@@ -26049,10 +26034,10 @@
         <v>1689</v>
       </c>
       <c r="I620" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J620" s="0" t="s">
-        <v>1690</v>
+        <v>1186</v>
       </c>
       <c r="K620" s="0" t="s">
         <v>326</v>
@@ -26063,7 +26048,7 @@
         <v>324</v>
       </c>
       <c r="B621" s="0" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="C621" s="0" t="s">
         <v>13</v>
@@ -26072,7 +26057,7 @@
         <v>325</v>
       </c>
       <c r="E621" s="0" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="F621" s="0" t="s">
         <v>348</v>
@@ -26081,13 +26066,13 @@
         <v>1423</v>
       </c>
       <c r="H621" s="0" t="s">
+        <v>1692</v>
+      </c>
+      <c r="I621" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="J621" s="0" t="s">
         <v>1693</v>
-      </c>
-      <c r="I621" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="J621" s="0" t="s">
-        <v>1186</v>
       </c>
       <c r="K621" s="0" t="s">
         <v>326</v>
@@ -26119,7 +26104,7 @@
         <v>1696</v>
       </c>
       <c r="I622" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J622" s="0" t="s">
         <v>1697</v>
@@ -26154,10 +26139,10 @@
         <v>1700</v>
       </c>
       <c r="I623" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J623" s="0" t="s">
-        <v>1701</v>
+        <v>1296</v>
       </c>
       <c r="K623" s="0" t="s">
         <v>326</v>
@@ -26168,7 +26153,7 @@
         <v>324</v>
       </c>
       <c r="B624" s="0" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="C624" s="0" t="s">
         <v>13</v>
@@ -26177,7 +26162,7 @@
         <v>325</v>
       </c>
       <c r="E624" s="0" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="F624" s="0" t="s">
         <v>348</v>
@@ -26186,13 +26171,13 @@
         <v>1423</v>
       </c>
       <c r="H624" s="0" t="s">
+        <v>1703</v>
+      </c>
+      <c r="I624" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="J624" s="0" t="s">
         <v>1704</v>
-      </c>
-      <c r="I624" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="J624" s="0" t="s">
-        <v>1296</v>
       </c>
       <c r="K624" s="0" t="s">
         <v>326</v>
@@ -26224,10 +26209,10 @@
         <v>1707</v>
       </c>
       <c r="I625" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J625" s="0" t="s">
-        <v>1708</v>
+        <v>1299</v>
       </c>
       <c r="K625" s="0" t="s">
         <v>326</v>
@@ -26238,7 +26223,7 @@
         <v>324</v>
       </c>
       <c r="B626" s="0" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="C626" s="0" t="s">
         <v>13</v>
@@ -26247,7 +26232,7 @@
         <v>325</v>
       </c>
       <c r="E626" s="0" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="F626" s="0" t="s">
         <v>348</v>
@@ -26256,13 +26241,13 @@
         <v>1423</v>
       </c>
       <c r="H626" s="0" t="s">
+        <v>1710</v>
+      </c>
+      <c r="I626" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="J626" s="0" t="s">
         <v>1711</v>
-      </c>
-      <c r="I626" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="J626" s="0" t="s">
-        <v>1299</v>
       </c>
       <c r="K626" s="0" t="s">
         <v>326</v>
@@ -26291,13 +26276,13 @@
         <v>1423</v>
       </c>
       <c r="H627" s="0" t="s">
+        <v>1707</v>
+      </c>
+      <c r="I627" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="J627" s="0" t="s">
         <v>1714</v>
-      </c>
-      <c r="I627" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="J627" s="0" t="s">
-        <v>1715</v>
       </c>
       <c r="K627" s="0" t="s">
         <v>326</v>
@@ -26308,7 +26293,7 @@
         <v>324</v>
       </c>
       <c r="B628" s="0" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="C628" s="0" t="s">
         <v>13</v>
@@ -26317,7 +26302,7 @@
         <v>325</v>
       </c>
       <c r="E628" s="0" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="F628" s="0" t="s">
         <v>348</v>
@@ -26326,10 +26311,10 @@
         <v>1423</v>
       </c>
       <c r="H628" s="0" t="s">
-        <v>1711</v>
+        <v>1717</v>
       </c>
       <c r="I628" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J628" s="0" t="s">
         <v>1718</v>
@@ -26364,7 +26349,7 @@
         <v>1721</v>
       </c>
       <c r="I629" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J629" s="0" t="s">
         <v>1722</v>
@@ -26399,7 +26384,7 @@
         <v>1725</v>
       </c>
       <c r="I630" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J630" s="0" t="s">
         <v>1726</v>
@@ -26434,7 +26419,7 @@
         <v>1729</v>
       </c>
       <c r="I631" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J631" s="0" t="s">
         <v>1730</v>
@@ -26469,7 +26454,7 @@
         <v>1733</v>
       </c>
       <c r="I632" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J632" s="0" t="s">
         <v>1734</v>
@@ -26504,7 +26489,7 @@
         <v>1737</v>
       </c>
       <c r="I633" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J633" s="0" t="s">
         <v>1738</v>
@@ -26530,7 +26515,7 @@
         <v>1740</v>
       </c>
       <c r="F634" s="0" t="s">
-        <v>348</v>
+        <v>28</v>
       </c>
       <c r="G634" s="0" t="s">
         <v>1423</v>
@@ -26539,7 +26524,7 @@
         <v>1741</v>
       </c>
       <c r="I634" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J634" s="0" t="s">
         <v>1742</v>
@@ -26565,7 +26550,7 @@
         <v>1744</v>
       </c>
       <c r="F635" s="0" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G635" s="0" t="s">
         <v>1423</v>
@@ -26574,7 +26559,7 @@
         <v>1745</v>
       </c>
       <c r="I635" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J635" s="0" t="s">
         <v>1746</v>
@@ -26600,7 +26585,7 @@
         <v>1748</v>
       </c>
       <c r="F636" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G636" s="0" t="s">
         <v>1423</v>
@@ -26609,7 +26594,7 @@
         <v>1749</v>
       </c>
       <c r="I636" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J636" s="0" t="s">
         <v>1750</v>
@@ -26644,7 +26629,7 @@
         <v>1753</v>
       </c>
       <c r="I637" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J637" s="0" t="s">
         <v>1754</v>
@@ -26670,7 +26655,7 @@
         <v>1756</v>
       </c>
       <c r="F638" s="0" t="s">
-        <v>28</v>
+        <v>348</v>
       </c>
       <c r="G638" s="0" t="s">
         <v>1423</v>
@@ -26679,7 +26664,7 @@
         <v>1757</v>
       </c>
       <c r="I638" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J638" s="0" t="s">
         <v>1758</v>
@@ -26705,7 +26690,7 @@
         <v>1760</v>
       </c>
       <c r="F639" s="0" t="s">
-        <v>348</v>
+        <v>153</v>
       </c>
       <c r="G639" s="0" t="s">
         <v>1423</v>
@@ -26714,7 +26699,7 @@
         <v>1761</v>
       </c>
       <c r="I639" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J639" s="0" t="s">
         <v>1762</v>
@@ -26749,7 +26734,7 @@
         <v>1765</v>
       </c>
       <c r="I640" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="J640" s="0" t="s">
         <v>1766</v>
@@ -26769,25 +26754,25 @@
         <v>13</v>
       </c>
       <c r="D641" s="0" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="E641" s="0" t="s">
         <v>1768</v>
       </c>
       <c r="F641" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="G641" s="0" t="s">
-        <v>1423</v>
+        <v>378</v>
+      </c>
+      <c r="G641" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H641" s="0" t="s">
         <v>1769</v>
       </c>
       <c r="I641" s="0" t="s">
-        <v>1581</v>
+        <v>380</v>
       </c>
       <c r="J641" s="0" t="s">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="K641" s="0" t="s">
         <v>326</v>
@@ -26798,7 +26783,7 @@
         <v>324</v>
       </c>
       <c r="B642" s="0" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="C642" s="0" t="s">
         <v>13</v>
@@ -26807,7 +26792,7 @@
         <v>333</v>
       </c>
       <c r="E642" s="0" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="F642" s="0" t="s">
         <v>378</v>
@@ -26816,13 +26801,13 @@
         <v>0</v>
       </c>
       <c r="H642" s="0" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="I642" s="0" t="s">
         <v>380</v>
       </c>
       <c r="J642" s="0" t="s">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="K642" s="0" t="s">
         <v>326</v>
@@ -26880,7 +26865,7 @@
         <v>1779</v>
       </c>
       <c r="F644" s="0" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="G644" s="0" t="n">
         <v>0</v>
@@ -26892,7 +26877,7 @@
         <v>380</v>
       </c>
       <c r="J644" s="0" t="s">
-        <v>1781</v>
+        <v>1773</v>
       </c>
       <c r="K644" s="0" t="s">
         <v>326</v>
@@ -26903,7 +26888,7 @@
         <v>324</v>
       </c>
       <c r="B645" s="0" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="C645" s="0" t="s">
         <v>13</v>
@@ -26912,7 +26897,7 @@
         <v>333</v>
       </c>
       <c r="E645" s="0" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="F645" s="0" t="s">
         <v>391</v>
@@ -26921,13 +26906,13 @@
         <v>0</v>
       </c>
       <c r="H645" s="0" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="I645" s="0" t="s">
         <v>380</v>
       </c>
       <c r="J645" s="0" t="s">
-        <v>1777</v>
+        <v>1784</v>
       </c>
       <c r="K645" s="0" t="s">
         <v>326</v>
@@ -26938,7 +26923,7 @@
         <v>324</v>
       </c>
       <c r="B646" s="0" t="s">
-        <v>1785</v>
+        <v>389</v>
       </c>
       <c r="C646" s="0" t="s">
         <v>13</v>
@@ -26947,22 +26932,22 @@
         <v>333</v>
       </c>
       <c r="E646" s="0" t="s">
-        <v>1786</v>
+        <v>390</v>
       </c>
       <c r="F646" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="G646" s="0" t="n">
-        <v>0</v>
+      <c r="G646" s="0" t="s">
+        <v>1423</v>
       </c>
       <c r="H646" s="0" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="I646" s="0" t="s">
         <v>380</v>
       </c>
       <c r="J646" s="0" t="s">
-        <v>1788</v>
+        <v>390</v>
       </c>
       <c r="K646" s="0" t="s">
         <v>326</v>
@@ -26973,31 +26958,31 @@
         <v>324</v>
       </c>
       <c r="B647" s="0" t="s">
-        <v>389</v>
+        <v>1786</v>
       </c>
       <c r="C647" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D647" s="0" t="s">
-        <v>333</v>
+        <v>1787</v>
       </c>
       <c r="E647" s="0" t="s">
-        <v>390</v>
+        <v>1788</v>
       </c>
       <c r="F647" s="0" t="s">
-        <v>391</v>
+        <v>1789</v>
       </c>
       <c r="G647" s="0" t="s">
         <v>1423</v>
       </c>
       <c r="H647" s="0" t="s">
-        <v>1789</v>
+        <v>1790</v>
       </c>
       <c r="I647" s="0" t="s">
-        <v>380</v>
+        <v>239</v>
       </c>
       <c r="J647" s="0" t="s">
-        <v>390</v>
+        <v>1791</v>
       </c>
       <c r="K647" s="0" t="s">
         <v>326</v>
@@ -27008,25 +26993,25 @@
         <v>324</v>
       </c>
       <c r="B648" s="0" t="s">
-        <v>1790</v>
+        <v>1792</v>
       </c>
       <c r="C648" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D648" s="0" t="s">
-        <v>1791</v>
+        <v>1787</v>
       </c>
       <c r="E648" s="0" t="s">
-        <v>1792</v>
+        <v>1793</v>
       </c>
       <c r="F648" s="0" t="s">
-        <v>1793</v>
+        <v>1794</v>
       </c>
       <c r="G648" s="0" t="s">
         <v>1423</v>
       </c>
       <c r="H648" s="0" t="s">
-        <v>1794</v>
+        <v>1790</v>
       </c>
       <c r="I648" s="0" t="s">
         <v>239</v>
@@ -27038,98 +27023,98 @@
         <v>326</v>
       </c>
     </row>
-    <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A649" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="B649" s="0" t="s">
+    <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A650" s="0" t="s">
+        <v>926</v>
+      </c>
+      <c r="B650" s="0" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C650" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D650" s="0" t="s">
+        <v>879</v>
+      </c>
+      <c r="E650" s="0" t="s">
+        <v>1768</v>
+      </c>
+      <c r="F650" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="G650" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H650" s="2" t="s">
         <v>1796</v>
       </c>
-      <c r="C649" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D649" s="0" t="s">
-        <v>1791</v>
-      </c>
-      <c r="E649" s="0" t="s">
-        <v>1797</v>
-      </c>
-      <c r="F649" s="0" t="s">
-        <v>1798</v>
-      </c>
-      <c r="G649" s="0" t="s">
-        <v>1423</v>
-      </c>
-      <c r="H649" s="0" t="s">
-        <v>1794</v>
-      </c>
-      <c r="I649" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="J649" s="0" t="s">
-        <v>1799</v>
-      </c>
-      <c r="K649" s="0" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="I650" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J650" s="0" t="s">
+        <v>1768</v>
+      </c>
+      <c r="K650" s="0" t="s">
+        <v>731</v>
+      </c>
+    </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="0" t="s">
         <v>926</v>
       </c>
-      <c r="B651" s="0" t="s">
-        <v>1771</v>
-      </c>
-      <c r="C651" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D651" s="0" t="s">
-        <v>879</v>
-      </c>
-      <c r="E651" s="0" t="s">
-        <v>1772</v>
-      </c>
-      <c r="F651" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="G651" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H651" s="2" t="s">
+      <c r="B651" s="3" t="s">
+        <v>1797</v>
+      </c>
+      <c r="H651" s="0" t="s">
+        <v>1798</v>
+      </c>
+      <c r="I651" s="0" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A653" s="0" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B653" s="0" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C653" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D653" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E653" s="0" t="s">
         <v>1800</v>
       </c>
-      <c r="I651" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="J651" s="0" t="s">
-        <v>1772</v>
-      </c>
-      <c r="K651" s="0" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A652" s="0" t="s">
-        <v>926</v>
-      </c>
-      <c r="B652" s="3" t="s">
+      <c r="F653" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="G653" s="0" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H653" s="0" t="s">
         <v>1801</v>
       </c>
-      <c r="H652" s="0" t="s">
+      <c r="I653" s="0" t="s">
         <v>1802</v>
       </c>
-      <c r="I652" s="0" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="J653" s="0" t="s">
+        <v>1803</v>
+      </c>
+      <c r="K653" s="0" t="s">
+        <v>1005</v>
+      </c>
+    </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="0" t="s">
         <v>1044</v>
       </c>
       <c r="B654" s="0" t="s">
-        <v>1803</v>
+        <v>1804</v>
       </c>
       <c r="C654" s="0" t="s">
         <v>13</v>
@@ -27138,7 +27123,7 @@
         <v>151</v>
       </c>
       <c r="E654" s="0" t="s">
-        <v>1804</v>
+        <v>1805</v>
       </c>
       <c r="F654" s="0" t="s">
         <v>153</v>
@@ -27147,13 +27132,13 @@
         <v>1423</v>
       </c>
       <c r="H654" s="0" t="s">
-        <v>1805</v>
+        <v>1801</v>
       </c>
       <c r="I654" s="0" t="s">
+        <v>1802</v>
+      </c>
+      <c r="J654" s="0" t="s">
         <v>1806</v>
-      </c>
-      <c r="J654" s="0" t="s">
-        <v>1807</v>
       </c>
       <c r="K654" s="0" t="s">
         <v>1005</v>
@@ -27164,7 +27149,7 @@
         <v>1044</v>
       </c>
       <c r="B655" s="0" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="C655" s="0" t="s">
         <v>13</v>
@@ -27173,7 +27158,7 @@
         <v>151</v>
       </c>
       <c r="E655" s="0" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="F655" s="0" t="s">
         <v>153</v>
@@ -27182,164 +27167,164 @@
         <v>1423</v>
       </c>
       <c r="H655" s="0" t="s">
-        <v>1805</v>
+        <v>1801</v>
       </c>
       <c r="I655" s="0" t="s">
-        <v>1806</v>
+        <v>1802</v>
       </c>
       <c r="J655" s="0" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="K655" s="0" t="s">
         <v>1005</v>
       </c>
     </row>
-    <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A656" s="0" t="s">
-        <v>1044</v>
-      </c>
-      <c r="B656" s="0" t="s">
+    <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A657" s="0" t="s">
+        <v>960</v>
+      </c>
+      <c r="B657" s="0" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C657" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D657" s="0" t="s">
+        <v>966</v>
+      </c>
+      <c r="E657" s="0" t="s">
         <v>1811</v>
       </c>
-      <c r="C656" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D656" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="E656" s="0" t="s">
+      <c r="F657" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G657" s="0" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H657" s="0" t="s">
         <v>1812</v>
       </c>
-      <c r="F656" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="G656" s="0" t="s">
-        <v>1423</v>
-      </c>
-      <c r="H656" s="0" t="s">
-        <v>1805</v>
-      </c>
-      <c r="I656" s="0" t="s">
-        <v>1806</v>
-      </c>
-      <c r="J656" s="0" t="s">
+      <c r="I657" s="0" t="s">
         <v>1813</v>
       </c>
-      <c r="K656" s="0" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="J657" s="0" t="s">
+        <v>1814</v>
+      </c>
+      <c r="K657" s="0" t="s">
+        <v>1815</v>
+      </c>
+    </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="0" t="s">
         <v>960</v>
       </c>
       <c r="B658" s="0" t="s">
-        <v>1814</v>
+        <v>1816</v>
       </c>
       <c r="C658" s="0" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D658" s="0" t="s">
         <v>966</v>
       </c>
       <c r="E658" s="0" t="s">
-        <v>1815</v>
+        <v>1817</v>
       </c>
       <c r="F658" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G658" s="0" t="s">
         <v>1423</v>
       </c>
       <c r="H658" s="0" t="s">
-        <v>1816</v>
+        <v>1818</v>
       </c>
       <c r="I658" s="0" t="s">
-        <v>1817</v>
+        <v>1813</v>
       </c>
       <c r="J658" s="0" t="s">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="K658" s="0" t="s">
-        <v>1819</v>
-      </c>
-    </row>
-    <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A659" s="0" t="s">
-        <v>960</v>
-      </c>
-      <c r="B659" s="0" t="s">
         <v>1820</v>
       </c>
-      <c r="C659" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D659" s="0" t="s">
-        <v>966</v>
-      </c>
-      <c r="E659" s="0" t="s">
+    </row>
+    <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A660" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="B660" s="0" t="s">
         <v>1821</v>
       </c>
-      <c r="F659" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G659" s="0" t="s">
+      <c r="C660" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D660" s="0" t="s">
+        <v>879</v>
+      </c>
+      <c r="E660" s="0" t="s">
+        <v>1822</v>
+      </c>
+      <c r="F660" s="0" t="s">
+        <v>734</v>
+      </c>
+      <c r="G660" s="0" t="s">
         <v>1423</v>
       </c>
-      <c r="H659" s="0" t="s">
+      <c r="H660" s="0" t="s">
+        <v>1823</v>
+      </c>
+      <c r="I660" s="0" t="s">
+        <v>994</v>
+      </c>
+      <c r="J660" s="0" t="s">
+        <v>747</v>
+      </c>
+      <c r="K660" s="0" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A662" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="B662" s="0" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C662" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D662" s="0" t="s">
+        <v>744</v>
+      </c>
+      <c r="E662" s="0" t="s">
         <v>1822</v>
       </c>
-      <c r="I659" s="0" t="s">
-        <v>1817</v>
-      </c>
-      <c r="J659" s="0" t="s">
-        <v>1823</v>
-      </c>
-      <c r="K659" s="0" t="s">
-        <v>1824</v>
-      </c>
-    </row>
-    <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A661" s="0" t="s">
-        <v>974</v>
-      </c>
-      <c r="B661" s="0" t="s">
-        <v>1525</v>
-      </c>
-      <c r="C661" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D661" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="E661" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="F661" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="G661" s="0" t="s">
+      <c r="F662" s="0" t="s">
+        <v>734</v>
+      </c>
+      <c r="G662" s="0" t="s">
         <v>1423</v>
       </c>
-      <c r="H661" s="0" t="s">
-        <v>1141</v>
-      </c>
-      <c r="I661" s="0" t="s">
-        <v>1527</v>
-      </c>
-      <c r="J661" s="0" t="s">
-        <v>1528</v>
-      </c>
-      <c r="K661" s="0" t="s">
+      <c r="H662" s="0" t="s">
         <v>1825</v>
       </c>
-    </row>
-    <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="I662" s="0" t="s">
+        <v>994</v>
+      </c>
+      <c r="J662" s="0" t="s">
+        <v>747</v>
+      </c>
+      <c r="K662" s="0" t="s">
+        <v>741</v>
+      </c>
+    </row>
     <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="0" t="s">
-        <v>856</v>
+        <v>740</v>
       </c>
       <c r="B663" s="0" t="s">
         <v>1826</v>
@@ -27348,7 +27333,7 @@
         <v>13</v>
       </c>
       <c r="D663" s="0" t="s">
-        <v>879</v>
+        <v>744</v>
       </c>
       <c r="E663" s="0" t="s">
         <v>1827</v>
@@ -27356,242 +27341,242 @@
       <c r="F663" s="0" t="s">
         <v>734</v>
       </c>
-      <c r="G663" s="0" t="s">
-        <v>1423</v>
+      <c r="G663" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H663" s="0" t="s">
         <v>1828</v>
       </c>
       <c r="I663" s="0" t="s">
-        <v>994</v>
+        <v>1577</v>
       </c>
       <c r="J663" s="0" t="s">
         <v>747</v>
       </c>
       <c r="K663" s="0" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A665" s="0" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A664" s="0" t="s">
         <v>740</v>
       </c>
-      <c r="B665" s="0" t="s">
+      <c r="B664" s="0" t="s">
         <v>1829</v>
       </c>
-      <c r="C665" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D665" s="0" t="s">
-        <v>744</v>
-      </c>
-      <c r="E665" s="0" t="s">
-        <v>1827</v>
-      </c>
-      <c r="F665" s="0" t="s">
-        <v>734</v>
-      </c>
-      <c r="G665" s="0" t="s">
-        <v>1423</v>
-      </c>
-      <c r="H665" s="0" t="s">
+      <c r="C664" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D664" s="0" t="s">
+        <v>750</v>
+      </c>
+      <c r="E664" s="0" t="s">
         <v>1830</v>
       </c>
-      <c r="I665" s="0" t="s">
-        <v>994</v>
-      </c>
-      <c r="J665" s="0" t="s">
-        <v>747</v>
-      </c>
-      <c r="K665" s="0" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A666" s="0" t="s">
-        <v>740</v>
-      </c>
-      <c r="B666" s="0" t="s">
-        <v>1831</v>
-      </c>
-      <c r="C666" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D666" s="0" t="s">
-        <v>744</v>
-      </c>
-      <c r="E666" s="0" t="s">
-        <v>1832</v>
-      </c>
-      <c r="F666" s="0" t="s">
-        <v>734</v>
-      </c>
-      <c r="G666" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H666" s="0" t="s">
-        <v>1833</v>
-      </c>
-      <c r="I666" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="J666" s="0" t="s">
-        <v>747</v>
-      </c>
-      <c r="K666" s="0" t="s">
+      <c r="F664" s="0" t="s">
+        <v>768</v>
+      </c>
+      <c r="G664" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H664" s="0" t="s">
+        <v>1828</v>
+      </c>
+      <c r="I664" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="J664" s="0" t="s">
+        <v>1830</v>
+      </c>
+      <c r="K664" s="0" t="s">
         <v>748</v>
       </c>
     </row>
+    <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="0" t="s">
-        <v>740</v>
+        <v>457</v>
       </c>
       <c r="B667" s="0" t="s">
-        <v>1834</v>
+        <v>389</v>
       </c>
       <c r="C667" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D667" s="0" t="s">
-        <v>750</v>
+        <v>459</v>
       </c>
       <c r="E667" s="0" t="s">
-        <v>1835</v>
+        <v>390</v>
       </c>
       <c r="F667" s="0" t="s">
-        <v>768</v>
-      </c>
-      <c r="G667" s="0" t="n">
-        <v>0</v>
+        <v>391</v>
+      </c>
+      <c r="G667" s="0" t="s">
+        <v>1423</v>
       </c>
       <c r="H667" s="0" t="s">
-        <v>1833</v>
+        <v>392</v>
       </c>
       <c r="I667" s="0" t="s">
-        <v>1581</v>
+        <v>380</v>
       </c>
       <c r="J667" s="0" t="s">
-        <v>1835</v>
+        <v>390</v>
       </c>
       <c r="K667" s="0" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A670" s="0" t="s">
-        <v>457</v>
-      </c>
-      <c r="B670" s="0" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A668" s="0" t="s">
+        <v>926</v>
+      </c>
+      <c r="B668" s="0" t="s">
         <v>389</v>
       </c>
-      <c r="C670" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D670" s="0" t="s">
-        <v>459</v>
-      </c>
-      <c r="E670" s="0" t="s">
+      <c r="C668" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D668" s="0" t="s">
+        <v>879</v>
+      </c>
+      <c r="E668" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="F670" s="0" t="s">
+      <c r="F668" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="G670" s="0" t="s">
+      <c r="G668" s="0" t="s">
         <v>1423</v>
       </c>
-      <c r="H670" s="0" t="s">
+      <c r="H668" s="0" t="s">
         <v>392</v>
       </c>
-      <c r="I670" s="0" t="s">
+      <c r="I668" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="J670" s="0" t="s">
+      <c r="J668" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="K670" s="0" t="s">
-        <v>462</v>
-      </c>
-    </row>
+      <c r="K668" s="0" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A669" s="0" t="s">
+        <v>926</v>
+      </c>
+      <c r="B669" s="0" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C669" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D669" s="0" t="s">
+        <v>879</v>
+      </c>
+      <c r="E669" s="0" t="s">
+        <v>1768</v>
+      </c>
+      <c r="F669" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="G669" s="0" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H669" s="0" t="s">
+        <v>1831</v>
+      </c>
+      <c r="I669" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="J669" s="0" t="s">
+        <v>1768</v>
+      </c>
+      <c r="K669" s="0" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="0" t="s">
-        <v>926</v>
+        <v>1052</v>
       </c>
       <c r="B671" s="0" t="s">
-        <v>389</v>
+        <v>1139</v>
       </c>
       <c r="C671" s="0" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="D671" s="0" t="s">
-        <v>879</v>
+        <v>151</v>
       </c>
       <c r="E671" s="0" t="s">
-        <v>390</v>
+        <v>1140</v>
       </c>
       <c r="F671" s="0" t="s">
-        <v>391</v>
+        <v>153</v>
       </c>
       <c r="G671" s="0" t="s">
         <v>1423</v>
       </c>
       <c r="H671" s="0" t="s">
-        <v>392</v>
+        <v>1141</v>
       </c>
       <c r="I671" s="0" t="s">
-        <v>380</v>
+        <v>1142</v>
       </c>
       <c r="J671" s="0" t="s">
-        <v>390</v>
+        <v>1143</v>
       </c>
       <c r="K671" s="0" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A672" s="0" t="s">
-        <v>926</v>
-      </c>
-      <c r="B672" s="0" t="s">
-        <v>1771</v>
-      </c>
-      <c r="C672" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D672" s="0" t="s">
-        <v>879</v>
-      </c>
-      <c r="E672" s="0" t="s">
-        <v>1772</v>
-      </c>
-      <c r="F672" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="G672" s="0" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A673" s="0" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B673" s="0" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C673" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D673" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E673" s="0" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F673" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="G673" s="0" t="s">
         <v>1423</v>
       </c>
-      <c r="H672" s="0" t="s">
-        <v>1836</v>
-      </c>
-      <c r="I672" s="0" t="s">
-        <v>380</v>
-      </c>
-      <c r="J672" s="0" t="s">
-        <v>1772</v>
-      </c>
-      <c r="K672" s="0" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H673" s="0" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I673" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J673" s="0" t="s">
+        <v>775</v>
+      </c>
+      <c r="K673" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="0" t="s">
-        <v>1052</v>
+        <v>974</v>
       </c>
       <c r="B674" s="0" t="s">
-        <v>1139</v>
+        <v>1049</v>
       </c>
       <c r="C674" s="0" t="s">
         <v>13</v>
@@ -27600,7 +27585,7 @@
         <v>151</v>
       </c>
       <c r="E674" s="0" t="s">
-        <v>1140</v>
+        <v>1832</v>
       </c>
       <c r="F674" s="0" t="s">
         <v>153</v>
@@ -27609,69 +27594,35 @@
         <v>1423</v>
       </c>
       <c r="H674" s="0" t="s">
-        <v>1141</v>
+        <v>1051</v>
       </c>
       <c r="I674" s="0" t="s">
-        <v>1142</v>
+        <v>56</v>
       </c>
       <c r="J674" s="0" t="s">
-        <v>1143</v>
+        <v>775</v>
       </c>
       <c r="K674" s="0" t="s">
-        <v>1083</v>
+        <v>20</v>
       </c>
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A676" s="0" t="s">
-        <v>1044</v>
-      </c>
-      <c r="B676" s="0" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C676" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D676" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="E676" s="0" t="s">
-        <v>1050</v>
-      </c>
-      <c r="F676" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="G676" s="0" t="s">
-        <v>1423</v>
-      </c>
-      <c r="H676" s="0" t="s">
-        <v>1051</v>
-      </c>
-      <c r="I676" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J676" s="0" t="s">
-        <v>775</v>
-      </c>
-      <c r="K676" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
+    <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="0" t="s">
-        <v>974</v>
+        <v>515</v>
       </c>
       <c r="B677" s="0" t="s">
-        <v>1049</v>
+        <v>1833</v>
       </c>
       <c r="C677" s="0" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D677" s="0" t="s">
         <v>151</v>
       </c>
       <c r="E677" s="0" t="s">
-        <v>1837</v>
+        <v>1834</v>
       </c>
       <c r="F677" s="0" t="s">
         <v>153</v>
@@ -27680,63 +27631,131 @@
         <v>1423</v>
       </c>
       <c r="H677" s="0" t="s">
-        <v>1051</v>
+        <v>1835</v>
       </c>
       <c r="I677" s="0" t="s">
-        <v>56</v>
+        <v>1836</v>
       </c>
       <c r="J677" s="0" t="s">
         <v>775</v>
       </c>
       <c r="K677" s="0" t="s">
-        <v>20</v>
+        <v>624</v>
       </c>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="0" t="s">
-        <v>515</v>
+        <v>974</v>
       </c>
       <c r="B680" s="0" t="s">
-        <v>1838</v>
-      </c>
-      <c r="C680" s="0" t="s">
-        <v>32</v>
+        <v>1496</v>
+      </c>
+      <c r="C680" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="D680" s="0" t="s">
         <v>151</v>
       </c>
       <c r="E680" s="0" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="F680" s="0" t="s">
-        <v>153</v>
+        <v>1498</v>
       </c>
       <c r="G680" s="0" t="s">
         <v>1423</v>
       </c>
       <c r="H680" s="0" t="s">
-        <v>1840</v>
+        <v>1463</v>
       </c>
       <c r="I680" s="0" t="s">
-        <v>1841</v>
+        <v>1464</v>
       </c>
       <c r="J680" s="0" t="s">
-        <v>775</v>
+        <v>1499</v>
       </c>
       <c r="K680" s="0" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A681" s="0" t="s">
+        <v>974</v>
+      </c>
+      <c r="B681" s="0" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C681" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D681" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E681" s="0" t="s">
+        <v>1838</v>
+      </c>
+      <c r="F681" s="0" t="s">
+        <v>1498</v>
+      </c>
+      <c r="G681" s="0" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H681" s="0" t="s">
+        <v>1463</v>
+      </c>
+      <c r="I681" s="0" t="s">
+        <v>1464</v>
+      </c>
+      <c r="J681" s="0" t="s">
+        <v>1502</v>
+      </c>
+      <c r="K681" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A682" s="0" t="s">
+        <v>974</v>
+      </c>
+      <c r="B682" s="0" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C682" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D682" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E682" s="0" t="s">
+        <v>1568</v>
+      </c>
+      <c r="F682" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="G682" s="0" t="s">
+        <v>1423</v>
+      </c>
+      <c r="H682" s="0" t="s">
+        <v>1463</v>
+      </c>
+      <c r="I682" s="0" t="s">
+        <v>1464</v>
+      </c>
+      <c r="J682" s="0" t="s">
+        <v>1569</v>
+      </c>
+      <c r="K682" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="0" t="s">
         <v>974</v>
       </c>
       <c r="B683" s="0" t="s">
-        <v>1496</v>
+        <v>1570</v>
       </c>
       <c r="C683" s="0" t="n">
         <v>1</v>
@@ -27745,10 +27764,10 @@
         <v>151</v>
       </c>
       <c r="E683" s="0" t="s">
-        <v>1842</v>
+        <v>1839</v>
       </c>
       <c r="F683" s="0" t="s">
-        <v>1498</v>
+        <v>852</v>
       </c>
       <c r="G683" s="0" t="s">
         <v>1423</v>
@@ -27760,7 +27779,7 @@
         <v>1464</v>
       </c>
       <c r="J683" s="0" t="s">
-        <v>1499</v>
+        <v>1572</v>
       </c>
       <c r="K683" s="0" t="s">
         <v>20</v>
@@ -27771,7 +27790,7 @@
         <v>974</v>
       </c>
       <c r="B684" s="0" t="s">
-        <v>1500</v>
+        <v>1461</v>
       </c>
       <c r="C684" s="0" t="n">
         <v>1</v>
@@ -27780,10 +27799,10 @@
         <v>151</v>
       </c>
       <c r="E684" s="0" t="s">
-        <v>1843</v>
-      </c>
-      <c r="F684" s="0" t="s">
-        <v>1498</v>
+        <v>1462</v>
+      </c>
+      <c r="F684" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G684" s="0" t="s">
         <v>1423</v>
@@ -27795,7 +27814,7 @@
         <v>1464</v>
       </c>
       <c r="J684" s="0" t="s">
-        <v>1502</v>
+        <v>1465</v>
       </c>
       <c r="K684" s="0" t="s">
         <v>20</v>
@@ -27806,7 +27825,7 @@
         <v>974</v>
       </c>
       <c r="B685" s="0" t="s">
-        <v>1571</v>
+        <v>1470</v>
       </c>
       <c r="C685" s="0" t="n">
         <v>1</v>
@@ -27815,10 +27834,10 @@
         <v>151</v>
       </c>
       <c r="E685" s="0" t="s">
-        <v>1572</v>
+        <v>1840</v>
       </c>
       <c r="F685" s="0" t="s">
-        <v>852</v>
+        <v>16</v>
       </c>
       <c r="G685" s="0" t="s">
         <v>1423</v>
@@ -27830,7 +27849,7 @@
         <v>1464</v>
       </c>
       <c r="J685" s="0" t="s">
-        <v>1573</v>
+        <v>1472</v>
       </c>
       <c r="K685" s="0" t="s">
         <v>20</v>
@@ -27841,7 +27860,7 @@
         <v>974</v>
       </c>
       <c r="B686" s="0" t="s">
-        <v>1574</v>
+        <v>1507</v>
       </c>
       <c r="C686" s="0" t="n">
         <v>1</v>
@@ -27850,10 +27869,10 @@
         <v>151</v>
       </c>
       <c r="E686" s="0" t="s">
-        <v>1844</v>
+        <v>1841</v>
       </c>
       <c r="F686" s="0" t="s">
-        <v>852</v>
+        <v>153</v>
       </c>
       <c r="G686" s="0" t="s">
         <v>1423</v>
@@ -27865,7 +27884,7 @@
         <v>1464</v>
       </c>
       <c r="J686" s="0" t="s">
-        <v>1576</v>
+        <v>1842</v>
       </c>
       <c r="K686" s="0" t="s">
         <v>20</v>
@@ -27876,7 +27895,7 @@
         <v>974</v>
       </c>
       <c r="B687" s="0" t="s">
-        <v>1461</v>
+        <v>1553</v>
       </c>
       <c r="C687" s="0" t="n">
         <v>1</v>
@@ -27885,10 +27904,10 @@
         <v>151</v>
       </c>
       <c r="E687" s="0" t="s">
-        <v>1462</v>
-      </c>
-      <c r="F687" s="0" t="n">
-        <v>1</v>
+        <v>1843</v>
+      </c>
+      <c r="F687" s="0" t="s">
+        <v>153</v>
       </c>
       <c r="G687" s="0" t="s">
         <v>1423</v>
@@ -27900,7 +27919,7 @@
         <v>1464</v>
       </c>
       <c r="J687" s="0" t="s">
-        <v>1465</v>
+        <v>1844</v>
       </c>
       <c r="K687" s="0" t="s">
         <v>20</v>
@@ -27911,7 +27930,7 @@
         <v>974</v>
       </c>
       <c r="B688" s="0" t="s">
-        <v>1470</v>
+        <v>1487</v>
       </c>
       <c r="C688" s="0" t="n">
         <v>1</v>
@@ -27923,7 +27942,7 @@
         <v>1845</v>
       </c>
       <c r="F688" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G688" s="0" t="s">
         <v>1423</v>
@@ -27935,7 +27954,7 @@
         <v>1464</v>
       </c>
       <c r="J688" s="0" t="s">
-        <v>1472</v>
+        <v>1489</v>
       </c>
       <c r="K688" s="0" t="s">
         <v>20</v>
@@ -27946,7 +27965,7 @@
         <v>974</v>
       </c>
       <c r="B689" s="0" t="s">
-        <v>1507</v>
+        <v>1490</v>
       </c>
       <c r="C689" s="0" t="n">
         <v>1</v>
@@ -27958,7 +27977,7 @@
         <v>1846</v>
       </c>
       <c r="F689" s="0" t="s">
-        <v>153</v>
+        <v>28</v>
       </c>
       <c r="G689" s="0" t="s">
         <v>1423</v>
@@ -27981,7 +28000,7 @@
         <v>974</v>
       </c>
       <c r="B690" s="0" t="s">
-        <v>1557</v>
+        <v>1493</v>
       </c>
       <c r="C690" s="0" t="n">
         <v>1</v>
@@ -27990,10 +28009,10 @@
         <v>151</v>
       </c>
       <c r="E690" s="0" t="s">
-        <v>1848</v>
+        <v>1494</v>
       </c>
       <c r="F690" s="0" t="s">
-        <v>153</v>
+        <v>28</v>
       </c>
       <c r="G690" s="0" t="s">
         <v>1423</v>
@@ -28005,7 +28024,7 @@
         <v>1464</v>
       </c>
       <c r="J690" s="0" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="K690" s="0" t="s">
         <v>20</v>
@@ -28016,7 +28035,7 @@
         <v>974</v>
       </c>
       <c r="B691" s="0" t="s">
-        <v>1487</v>
+        <v>1473</v>
       </c>
       <c r="C691" s="0" t="n">
         <v>1</v>
@@ -28025,7 +28044,7 @@
         <v>151</v>
       </c>
       <c r="E691" s="0" t="s">
-        <v>1850</v>
+        <v>1474</v>
       </c>
       <c r="F691" s="0" t="s">
         <v>28</v>
@@ -28040,7 +28059,7 @@
         <v>1464</v>
       </c>
       <c r="J691" s="0" t="s">
-        <v>1489</v>
+        <v>1475</v>
       </c>
       <c r="K691" s="0" t="s">
         <v>20</v>
@@ -28051,7 +28070,7 @@
         <v>974</v>
       </c>
       <c r="B692" s="0" t="s">
-        <v>1490</v>
+        <v>1547</v>
       </c>
       <c r="C692" s="0" t="n">
         <v>1</v>
@@ -28060,7 +28079,7 @@
         <v>151</v>
       </c>
       <c r="E692" s="0" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="F692" s="0" t="s">
         <v>28</v>
@@ -28075,7 +28094,7 @@
         <v>1464</v>
       </c>
       <c r="J692" s="0" t="s">
-        <v>1852</v>
+        <v>1549</v>
       </c>
       <c r="K692" s="0" t="s">
         <v>20</v>
@@ -28086,7 +28105,7 @@
         <v>974</v>
       </c>
       <c r="B693" s="0" t="s">
-        <v>1493</v>
+        <v>1212</v>
       </c>
       <c r="C693" s="0" t="n">
         <v>1</v>
@@ -28095,7 +28114,7 @@
         <v>151</v>
       </c>
       <c r="E693" s="0" t="s">
-        <v>1494</v>
+        <v>1213</v>
       </c>
       <c r="F693" s="0" t="s">
         <v>28</v>
@@ -28110,7 +28129,7 @@
         <v>1464</v>
       </c>
       <c r="J693" s="0" t="s">
-        <v>1853</v>
+        <v>1216</v>
       </c>
       <c r="K693" s="0" t="s">
         <v>20</v>
@@ -28121,19 +28140,19 @@
         <v>974</v>
       </c>
       <c r="B694" s="0" t="s">
-        <v>1473</v>
+        <v>1522</v>
       </c>
       <c r="C694" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D694" s="0" t="s">
-        <v>151</v>
+        <v>1001</v>
       </c>
       <c r="E694" s="0" t="s">
-        <v>1474</v>
-      </c>
-      <c r="F694" s="0" t="s">
-        <v>28</v>
+        <v>1850</v>
+      </c>
+      <c r="F694" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G694" s="0" t="s">
         <v>1423</v>
@@ -28145,7 +28164,7 @@
         <v>1464</v>
       </c>
       <c r="J694" s="0" t="s">
-        <v>1475</v>
+        <v>1524</v>
       </c>
       <c r="K694" s="0" t="s">
         <v>20</v>
@@ -28156,19 +28175,19 @@
         <v>974</v>
       </c>
       <c r="B695" s="0" t="s">
-        <v>1551</v>
+        <v>1519</v>
       </c>
       <c r="C695" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D695" s="0" t="s">
-        <v>151</v>
+        <v>1001</v>
       </c>
       <c r="E695" s="0" t="s">
-        <v>1854</v>
-      </c>
-      <c r="F695" s="0" t="s">
-        <v>28</v>
+        <v>1851</v>
+      </c>
+      <c r="F695" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="G695" s="0" t="s">
         <v>1423</v>
@@ -28180,7 +28199,7 @@
         <v>1464</v>
       </c>
       <c r="J695" s="0" t="s">
-        <v>1553</v>
+        <v>1521</v>
       </c>
       <c r="K695" s="0" t="s">
         <v>20</v>
@@ -28191,19 +28210,19 @@
         <v>974</v>
       </c>
       <c r="B696" s="0" t="s">
-        <v>1212</v>
+        <v>1480</v>
       </c>
       <c r="C696" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D696" s="0" t="s">
-        <v>151</v>
+        <v>1481</v>
       </c>
       <c r="E696" s="0" t="s">
-        <v>1213</v>
+        <v>1852</v>
       </c>
       <c r="F696" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="G696" s="0" t="s">
         <v>1423</v>
@@ -28215,7 +28234,7 @@
         <v>1464</v>
       </c>
       <c r="J696" s="0" t="s">
-        <v>1216</v>
+        <v>1483</v>
       </c>
       <c r="K696" s="0" t="s">
         <v>20</v>
@@ -28226,19 +28245,19 @@
         <v>974</v>
       </c>
       <c r="B697" s="0" t="s">
-        <v>1522</v>
+        <v>1466</v>
       </c>
       <c r="C697" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D697" s="0" t="s">
-        <v>1001</v>
+        <v>151</v>
       </c>
       <c r="E697" s="0" t="s">
-        <v>1855</v>
-      </c>
-      <c r="F697" s="0" t="n">
-        <v>1</v>
+        <v>1853</v>
+      </c>
+      <c r="F697" s="0" t="s">
+        <v>1468</v>
       </c>
       <c r="G697" s="0" t="s">
         <v>1423</v>
@@ -28250,7 +28269,7 @@
         <v>1464</v>
       </c>
       <c r="J697" s="0" t="s">
-        <v>1524</v>
+        <v>1469</v>
       </c>
       <c r="K697" s="0" t="s">
         <v>20</v>
@@ -28261,19 +28280,19 @@
         <v>974</v>
       </c>
       <c r="B698" s="0" t="s">
-        <v>1519</v>
+        <v>1525</v>
       </c>
       <c r="C698" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D698" s="0" t="s">
-        <v>1001</v>
+        <v>151</v>
       </c>
       <c r="E698" s="0" t="s">
-        <v>1856</v>
-      </c>
-      <c r="F698" s="0" t="n">
-        <v>1</v>
+        <v>1854</v>
+      </c>
+      <c r="F698" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="G698" s="0" t="s">
         <v>1423</v>
@@ -28285,7 +28304,7 @@
         <v>1464</v>
       </c>
       <c r="J698" s="0" t="s">
-        <v>1521</v>
+        <v>1855</v>
       </c>
       <c r="K698" s="0" t="s">
         <v>20</v>
@@ -28296,19 +28315,19 @@
         <v>974</v>
       </c>
       <c r="B699" s="0" t="s">
-        <v>1480</v>
+        <v>1528</v>
       </c>
       <c r="C699" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D699" s="0" t="s">
-        <v>1481</v>
+        <v>151</v>
       </c>
       <c r="E699" s="0" t="s">
-        <v>1857</v>
+        <v>1529</v>
       </c>
       <c r="F699" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G699" s="0" t="s">
         <v>1423</v>
@@ -28320,264 +28339,162 @@
         <v>1464</v>
       </c>
       <c r="J699" s="0" t="s">
-        <v>1483</v>
+        <v>1856</v>
       </c>
       <c r="K699" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A700" s="0" t="s">
-        <v>974</v>
-      </c>
-      <c r="B700" s="0" t="s">
-        <v>1466</v>
-      </c>
-      <c r="C700" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D700" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="E700" s="0" t="s">
-        <v>1858</v>
-      </c>
-      <c r="F700" s="0" t="s">
-        <v>1468</v>
-      </c>
-      <c r="G700" s="0" t="s">
-        <v>1423</v>
-      </c>
-      <c r="H700" s="0" t="s">
-        <v>1463</v>
-      </c>
-      <c r="I700" s="0" t="s">
-        <v>1464</v>
-      </c>
-      <c r="J700" s="0" t="s">
-        <v>1469</v>
-      </c>
-      <c r="K700" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
+    <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A701" s="0" t="s">
-        <v>974</v>
+        <v>856</v>
       </c>
       <c r="B701" s="0" t="s">
-        <v>1529</v>
-      </c>
-      <c r="C701" s="0" t="n">
-        <v>1</v>
+        <v>1857</v>
+      </c>
+      <c r="C701" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="D701" s="0" t="s">
-        <v>151</v>
+        <v>896</v>
       </c>
       <c r="E701" s="0" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F701" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="G701" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H701" s="2" t="s">
         <v>1859</v>
       </c>
-      <c r="F701" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G701" s="0" t="s">
-        <v>1423</v>
-      </c>
-      <c r="H701" s="0" t="s">
-        <v>1463</v>
-      </c>
       <c r="I701" s="0" t="s">
-        <v>1464</v>
+        <v>56</v>
       </c>
       <c r="J701" s="0" t="s">
         <v>1860</v>
       </c>
       <c r="K701" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A702" s="0" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A703" s="2" t="s">
         <v>974</v>
       </c>
-      <c r="B702" s="0" t="s">
-        <v>1532</v>
-      </c>
-      <c r="C702" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D702" s="0" t="s">
+      <c r="B703" s="2" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C703" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D703" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E702" s="0" t="s">
-        <v>1533</v>
-      </c>
-      <c r="F702" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G702" s="0" t="s">
-        <v>1423</v>
-      </c>
-      <c r="H702" s="0" t="s">
-        <v>1463</v>
-      </c>
-      <c r="I702" s="0" t="s">
-        <v>1464</v>
-      </c>
-      <c r="J702" s="0" t="s">
-        <v>1861</v>
-      </c>
-      <c r="K702" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A704" s="0" t="s">
-        <v>856</v>
-      </c>
-      <c r="B704" s="0" t="s">
+      <c r="E703" s="2" t="s">
         <v>1862</v>
       </c>
-      <c r="C704" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D704" s="0" t="s">
-        <v>896</v>
-      </c>
-      <c r="E704" s="0" t="s">
-        <v>1863</v>
-      </c>
-      <c r="F704" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="G704" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H704" s="2" t="s">
-        <v>1864</v>
-      </c>
-      <c r="I704" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J704" s="0" t="s">
-        <v>1865</v>
-      </c>
-      <c r="K704" s="0" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A706" s="2" t="s">
-        <v>974</v>
-      </c>
-      <c r="B706" s="2" t="s">
-        <v>1866</v>
-      </c>
-      <c r="C706" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D706" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E706" s="2" t="s">
-        <v>1867</v>
-      </c>
-      <c r="F706" s="2" t="s">
+      <c r="F703" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G706" s="2" t="str">
+      <c r="G703" s="2" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f0bf4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H706" s="2" t="s">
-        <v>1868</v>
-      </c>
-      <c r="I706" s="2" t="s">
-        <v>1869</v>
-      </c>
-      <c r="J706" s="2" t="s">
-        <v>1870</v>
-      </c>
-      <c r="K706" s="2" t="s">
+      <c r="H703" s="2" t="s">
+        <v>1863</v>
+      </c>
+      <c r="I703" s="2" t="s">
+        <v>1864</v>
+      </c>
+      <c r="J703" s="2" t="s">
+        <v>1865</v>
+      </c>
+      <c r="K703" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A708" s="0" t="s">
+    <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A705" s="0" t="s">
         <v>782</v>
       </c>
-      <c r="B708" s="0" t="s">
-        <v>1871</v>
-      </c>
-      <c r="C708" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D708" s="0" t="s">
+      <c r="B705" s="0" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C705" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D705" s="0" t="s">
         <v>459</v>
       </c>
-      <c r="E708" s="0" t="s">
+      <c r="E705" s="0" t="s">
         <v>745</v>
       </c>
-      <c r="F708" s="0" t="s">
+      <c r="F705" s="0" t="s">
         <v>734</v>
       </c>
-      <c r="G708" s="0" t="str">
+      <c r="G705" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9bb9a503065dfbd30c9bbe5c3c6abf99.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H708" s="0" t="s">
-        <v>1872</v>
-      </c>
-      <c r="I708" s="0" t="s">
+      <c r="H705" s="0" t="s">
+        <v>1867</v>
+      </c>
+      <c r="I705" s="0" t="s">
         <v>343</v>
       </c>
-      <c r="J708" s="0" t="s">
+      <c r="J705" s="0" t="s">
         <v>747</v>
       </c>
-      <c r="K708" s="0" t="s">
+      <c r="K705" s="0" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A709" s="0" t="s">
+    <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A706" s="0" t="s">
         <v>856</v>
       </c>
-      <c r="B709" s="0" t="s">
-        <v>1871</v>
-      </c>
-      <c r="C709" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D709" s="0" t="s">
+      <c r="B706" s="0" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C706" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D706" s="0" t="s">
         <v>879</v>
       </c>
-      <c r="E709" s="0" t="s">
+      <c r="E706" s="0" t="s">
         <v>745</v>
       </c>
-      <c r="F709" s="0" t="s">
+      <c r="F706" s="0" t="s">
         <v>734</v>
       </c>
-      <c r="G709" s="0" t="str">
+      <c r="G706" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9bb9a503065dfbd30c9bbe5c3c6abf99.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H709" s="0" t="s">
-        <v>1872</v>
-      </c>
-      <c r="I709" s="0" t="s">
+      <c r="H706" s="0" t="s">
+        <v>1867</v>
+      </c>
+      <c r="I706" s="0" t="s">
         <v>343</v>
       </c>
-      <c r="J709" s="0" t="s">
+      <c r="J706" s="0" t="s">
         <v>747</v>
       </c>
-      <c r="K709" s="0" t="s">
+      <c r="K706" s="0" t="s">
         <v>862</v>
       </c>
     </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>